<commit_message>
Added register button and register features
register button addition, with register fields, also specified specific css files for specific pages
</commit_message>
<xml_diff>
--- a/Documents/Timeline Plan.xlsx
+++ b/Documents/Timeline Plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Desktop\Software Engineering\Year 3\Final Year Project\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98BA2F79-1A31-46F1-B4CA-B9BDA93EB1ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C1118A0-629F-472F-8372-7AC3E1BED1F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{502DC14A-D437-40F5-AA7D-619030A61E6A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{502DC14A-D437-40F5-AA7D-619030A61E6A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -263,7 +263,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -534,11 +534,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -546,13 +585,7 @@
     <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -565,9 +598,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -586,83 +616,110 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1040,8 +1097,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEBB45B1-5618-49AC-BEB2-5915F2B48512}">
   <dimension ref="A1:AL44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:AL20"/>
+    <sheetView tabSelected="1" zoomScale="76" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="D33" sqref="A1:D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1054,130 +1111,130 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="J1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="16" t="s">
+      <c r="K1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="16" t="s">
+      <c r="L1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="16" t="s">
+      <c r="M1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="16" t="s">
+      <c r="N1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="16" t="s">
+      <c r="O1" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="16" t="s">
+      <c r="P1" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="16" t="s">
+      <c r="Q1" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="16" t="s">
+      <c r="R1" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="16" t="s">
+      <c r="S1" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="16" t="s">
+      <c r="T1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="16" t="s">
+      <c r="U1" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="V1" s="16" t="s">
+      <c r="V1" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="16" t="s">
+      <c r="W1" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="X1" s="16" t="s">
+      <c r="X1" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="Y1" s="16" t="s">
+      <c r="Y1" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="Z1" s="16" t="s">
+      <c r="Z1" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="AA1" s="16" t="s">
+      <c r="AA1" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="AB1" s="16" t="s">
+      <c r="AB1" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="AC1" s="16" t="s">
+      <c r="AC1" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="AD1" s="16" t="s">
+      <c r="AD1" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="AE1" s="16" t="s">
+      <c r="AE1" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="AF1" s="16" t="s">
+      <c r="AF1" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="AG1" s="16" t="s">
+      <c r="AG1" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="AH1" s="16" t="s">
+      <c r="AH1" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="AI1" s="16" t="s">
+      <c r="AI1" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="AJ1" s="16" t="s">
+      <c r="AJ1" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="AK1" s="16" t="s">
+      <c r="AK1" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="AL1" s="17" t="s">
+      <c r="AL1" s="14" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:38" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="3">
         <v>45194</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="F2" s="18" t="s">
+      <c r="D2" s="41"/>
+      <c r="F2" s="15" t="s">
         <v>3</v>
       </c>
       <c r="G2" s="2">
@@ -1273,993 +1330,998 @@
       <c r="AK2" s="2">
         <v>45404</v>
       </c>
-      <c r="AL2" s="19">
+      <c r="AL2" s="16">
         <v>45411</v>
       </c>
     </row>
     <row r="3" spans="1:38" ht="21" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>45201</v>
       </c>
-      <c r="C3" s="46" t="s">
+      <c r="C3" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="28"/>
-      <c r="F3" s="26" t="s">
+      <c r="D3" s="42"/>
+      <c r="F3" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="G3" s="37"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="6"/>
-      <c r="R3" s="6"/>
-      <c r="S3" s="6"/>
-      <c r="T3" s="6"/>
-      <c r="U3" s="6"/>
-      <c r="V3" s="6"/>
-      <c r="W3" s="6"/>
-      <c r="X3" s="6"/>
-      <c r="Y3" s="6"/>
-      <c r="Z3" s="6"/>
-      <c r="AA3" s="6"/>
-      <c r="AB3" s="6"/>
-      <c r="AC3" s="6"/>
-      <c r="AD3" s="6"/>
-      <c r="AE3" s="6"/>
-      <c r="AF3" s="6"/>
-      <c r="AG3" s="6"/>
-      <c r="AH3" s="6"/>
-      <c r="AI3" s="6"/>
-      <c r="AJ3" s="6"/>
-      <c r="AK3" s="6"/>
-      <c r="AL3" s="20"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4"/>
+      <c r="T3" s="4"/>
+      <c r="U3" s="4"/>
+      <c r="V3" s="4"/>
+      <c r="W3" s="4"/>
+      <c r="X3" s="4"/>
+      <c r="Y3" s="4"/>
+      <c r="Z3" s="4"/>
+      <c r="AA3" s="4"/>
+      <c r="AB3" s="4"/>
+      <c r="AC3" s="4"/>
+      <c r="AD3" s="4"/>
+      <c r="AE3" s="4"/>
+      <c r="AF3" s="4"/>
+      <c r="AG3" s="4"/>
+      <c r="AH3" s="4"/>
+      <c r="AI3" s="4"/>
+      <c r="AJ3" s="4"/>
+      <c r="AK3" s="4"/>
+      <c r="AL3" s="17"/>
     </row>
     <row r="4" spans="1:38" ht="21" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>45208</v>
       </c>
-      <c r="C4" s="46"/>
-      <c r="D4" s="29"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="6"/>
-      <c r="R4" s="6"/>
-      <c r="S4" s="6"/>
-      <c r="T4" s="6"/>
-      <c r="U4" s="6"/>
-      <c r="V4" s="6"/>
-      <c r="W4" s="6"/>
-      <c r="X4" s="6"/>
-      <c r="Y4" s="6"/>
-      <c r="Z4" s="6"/>
-      <c r="AA4" s="6"/>
-      <c r="AB4" s="6"/>
-      <c r="AC4" s="6"/>
-      <c r="AD4" s="6"/>
-      <c r="AE4" s="6"/>
-      <c r="AF4" s="6"/>
-      <c r="AG4" s="6"/>
-      <c r="AH4" s="6"/>
-      <c r="AI4" s="6"/>
-      <c r="AJ4" s="6"/>
-      <c r="AK4" s="6"/>
-      <c r="AL4" s="20"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="43"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
+      <c r="T4" s="4"/>
+      <c r="U4" s="4"/>
+      <c r="V4" s="4"/>
+      <c r="W4" s="4"/>
+      <c r="X4" s="4"/>
+      <c r="Y4" s="4"/>
+      <c r="Z4" s="4"/>
+      <c r="AA4" s="4"/>
+      <c r="AB4" s="4"/>
+      <c r="AC4" s="4"/>
+      <c r="AD4" s="4"/>
+      <c r="AE4" s="4"/>
+      <c r="AF4" s="4"/>
+      <c r="AG4" s="4"/>
+      <c r="AH4" s="4"/>
+      <c r="AI4" s="4"/>
+      <c r="AJ4" s="4"/>
+      <c r="AK4" s="4"/>
+      <c r="AL4" s="17"/>
     </row>
     <row r="5" spans="1:38" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <v>45215</v>
       </c>
-      <c r="C5" s="46"/>
-      <c r="D5" s="30"/>
-      <c r="F5" s="26" t="s">
+      <c r="C5" s="35"/>
+      <c r="D5" s="44"/>
+      <c r="F5" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="G5" s="6"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="6"/>
-      <c r="S5" s="6"/>
-      <c r="T5" s="6"/>
-      <c r="U5" s="6"/>
-      <c r="V5" s="6"/>
-      <c r="W5" s="6"/>
-      <c r="X5" s="6"/>
-      <c r="Y5" s="6"/>
-      <c r="Z5" s="6"/>
-      <c r="AA5" s="6"/>
-      <c r="AB5" s="6"/>
-      <c r="AC5" s="6"/>
-      <c r="AD5" s="6"/>
-      <c r="AE5" s="6"/>
-      <c r="AF5" s="6"/>
-      <c r="AG5" s="6"/>
-      <c r="AH5" s="6"/>
-      <c r="AI5" s="6"/>
-      <c r="AJ5" s="6"/>
-      <c r="AK5" s="6"/>
-      <c r="AL5" s="20"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
+      <c r="S5" s="4"/>
+      <c r="T5" s="4"/>
+      <c r="U5" s="4"/>
+      <c r="V5" s="4"/>
+      <c r="W5" s="4"/>
+      <c r="X5" s="4"/>
+      <c r="Y5" s="4"/>
+      <c r="Z5" s="4"/>
+      <c r="AA5" s="4"/>
+      <c r="AB5" s="4"/>
+      <c r="AC5" s="4"/>
+      <c r="AD5" s="4"/>
+      <c r="AE5" s="4"/>
+      <c r="AF5" s="4"/>
+      <c r="AG5" s="4"/>
+      <c r="AH5" s="4"/>
+      <c r="AI5" s="4"/>
+      <c r="AJ5" s="4"/>
+      <c r="AK5" s="4"/>
+      <c r="AL5" s="17"/>
     </row>
     <row r="6" spans="1:38" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="3">
         <v>45222</v>
       </c>
-      <c r="C6" s="46" t="s">
+      <c r="C6" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="34"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="6"/>
-      <c r="R6" s="6"/>
-      <c r="S6" s="6"/>
-      <c r="T6" s="6"/>
-      <c r="U6" s="6"/>
-      <c r="V6" s="6"/>
-      <c r="W6" s="6"/>
-      <c r="X6" s="6"/>
-      <c r="Y6" s="6"/>
-      <c r="Z6" s="6"/>
-      <c r="AA6" s="6"/>
-      <c r="AB6" s="6"/>
-      <c r="AC6" s="6"/>
-      <c r="AD6" s="6"/>
-      <c r="AE6" s="6"/>
-      <c r="AF6" s="6"/>
-      <c r="AG6" s="6"/>
-      <c r="AH6" s="6"/>
-      <c r="AI6" s="6"/>
-      <c r="AJ6" s="6"/>
-      <c r="AK6" s="6"/>
-      <c r="AL6" s="20"/>
+      <c r="D6" s="45"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4"/>
+      <c r="S6" s="4"/>
+      <c r="T6" s="4"/>
+      <c r="U6" s="4"/>
+      <c r="V6" s="4"/>
+      <c r="W6" s="4"/>
+      <c r="X6" s="4"/>
+      <c r="Y6" s="4"/>
+      <c r="Z6" s="4"/>
+      <c r="AA6" s="4"/>
+      <c r="AB6" s="4"/>
+      <c r="AC6" s="4"/>
+      <c r="AD6" s="4"/>
+      <c r="AE6" s="4"/>
+      <c r="AF6" s="4"/>
+      <c r="AG6" s="4"/>
+      <c r="AH6" s="4"/>
+      <c r="AI6" s="4"/>
+      <c r="AJ6" s="4"/>
+      <c r="AK6" s="4"/>
+      <c r="AL6" s="17"/>
     </row>
     <row r="7" spans="1:38" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="3">
         <v>45229</v>
       </c>
-      <c r="C7" s="46"/>
-      <c r="D7" s="35"/>
-      <c r="F7" s="26" t="s">
+      <c r="C7" s="35"/>
+      <c r="D7" s="46"/>
+      <c r="F7" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="G7" s="6"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="39"/>
-      <c r="L7" s="40"/>
-      <c r="M7" s="40"/>
-      <c r="N7" s="40"/>
-      <c r="O7" s="41"/>
-      <c r="P7" s="6"/>
-      <c r="Q7" s="6"/>
-      <c r="R7" s="6"/>
-      <c r="S7" s="6"/>
-      <c r="T7" s="6"/>
-      <c r="U7" s="6"/>
-      <c r="V7" s="6"/>
-      <c r="W7" s="6"/>
-      <c r="X7" s="6"/>
-      <c r="Y7" s="6"/>
-      <c r="Z7" s="6"/>
-      <c r="AA7" s="6"/>
-      <c r="AB7" s="6"/>
-      <c r="AC7" s="6"/>
-      <c r="AD7" s="6"/>
-      <c r="AE7" s="6"/>
-      <c r="AF7" s="6"/>
-      <c r="AG7" s="6"/>
-      <c r="AH7" s="6"/>
-      <c r="AI7" s="6"/>
-      <c r="AJ7" s="6"/>
-      <c r="AK7" s="6"/>
-      <c r="AL7" s="20"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="21"/>
+      <c r="M7" s="21"/>
+      <c r="N7" s="21"/>
+      <c r="O7" s="22"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="4"/>
+      <c r="S7" s="4"/>
+      <c r="T7" s="4"/>
+      <c r="U7" s="4"/>
+      <c r="V7" s="4"/>
+      <c r="W7" s="4"/>
+      <c r="X7" s="4"/>
+      <c r="Y7" s="4"/>
+      <c r="Z7" s="4"/>
+      <c r="AA7" s="4"/>
+      <c r="AB7" s="4"/>
+      <c r="AC7" s="4"/>
+      <c r="AD7" s="4"/>
+      <c r="AE7" s="4"/>
+      <c r="AF7" s="4"/>
+      <c r="AG7" s="4"/>
+      <c r="AH7" s="4"/>
+      <c r="AI7" s="4"/>
+      <c r="AJ7" s="4"/>
+      <c r="AK7" s="4"/>
+      <c r="AL7" s="17"/>
     </row>
     <row r="8" spans="1:38" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="3">
         <v>45236</v>
       </c>
-      <c r="C8" s="46"/>
-      <c r="D8" s="35"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="42"/>
-      <c r="L8" s="43"/>
-      <c r="M8" s="43"/>
-      <c r="N8" s="43"/>
-      <c r="O8" s="44"/>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="6"/>
-      <c r="R8" s="6"/>
-      <c r="S8" s="6"/>
-      <c r="T8" s="6"/>
-      <c r="U8" s="6"/>
-      <c r="V8" s="6"/>
-      <c r="W8" s="6"/>
-      <c r="X8" s="6"/>
-      <c r="Y8" s="6"/>
-      <c r="Z8" s="6"/>
-      <c r="AA8" s="6"/>
-      <c r="AB8" s="6"/>
-      <c r="AC8" s="6"/>
-      <c r="AD8" s="6"/>
-      <c r="AE8" s="6"/>
-      <c r="AF8" s="6"/>
-      <c r="AG8" s="6"/>
-      <c r="AH8" s="6"/>
-      <c r="AI8" s="6"/>
-      <c r="AJ8" s="6"/>
-      <c r="AK8" s="6"/>
-      <c r="AL8" s="20"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="46"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="24"/>
+      <c r="M8" s="24"/>
+      <c r="N8" s="24"/>
+      <c r="O8" s="25"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4"/>
+      <c r="R8" s="4"/>
+      <c r="S8" s="4"/>
+      <c r="T8" s="4"/>
+      <c r="U8" s="4"/>
+      <c r="V8" s="4"/>
+      <c r="W8" s="4"/>
+      <c r="X8" s="4"/>
+      <c r="Y8" s="4"/>
+      <c r="Z8" s="4"/>
+      <c r="AA8" s="4"/>
+      <c r="AB8" s="4"/>
+      <c r="AC8" s="4"/>
+      <c r="AD8" s="4"/>
+      <c r="AE8" s="4"/>
+      <c r="AF8" s="4"/>
+      <c r="AG8" s="4"/>
+      <c r="AH8" s="4"/>
+      <c r="AI8" s="4"/>
+      <c r="AJ8" s="4"/>
+      <c r="AK8" s="4"/>
+      <c r="AL8" s="17"/>
     </row>
     <row r="9" spans="1:38" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="3">
         <v>45243</v>
       </c>
-      <c r="C9" s="46"/>
-      <c r="D9" s="35"/>
-      <c r="F9" s="26" t="s">
+      <c r="C9" s="35"/>
+      <c r="D9" s="46"/>
+      <c r="F9" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
-      <c r="N9" s="13"/>
-      <c r="O9" s="13"/>
-      <c r="P9" s="39"/>
-      <c r="Q9" s="40"/>
-      <c r="R9" s="41"/>
-      <c r="S9" s="6"/>
-      <c r="T9" s="6"/>
-      <c r="U9" s="6"/>
-      <c r="V9" s="6"/>
-      <c r="W9" s="6"/>
-      <c r="X9" s="6"/>
-      <c r="Y9" s="6"/>
-      <c r="Z9" s="6"/>
-      <c r="AA9" s="6"/>
-      <c r="AB9" s="6"/>
-      <c r="AC9" s="6"/>
-      <c r="AD9" s="6"/>
-      <c r="AE9" s="6"/>
-      <c r="AF9" s="6"/>
-      <c r="AG9" s="6"/>
-      <c r="AH9" s="6"/>
-      <c r="AI9" s="6"/>
-      <c r="AJ9" s="6"/>
-      <c r="AK9" s="6"/>
-      <c r="AL9" s="20"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="20"/>
+      <c r="Q9" s="21"/>
+      <c r="R9" s="22"/>
+      <c r="S9" s="4"/>
+      <c r="T9" s="4"/>
+      <c r="U9" s="4"/>
+      <c r="V9" s="4"/>
+      <c r="W9" s="4"/>
+      <c r="X9" s="4"/>
+      <c r="Y9" s="4"/>
+      <c r="Z9" s="4"/>
+      <c r="AA9" s="4"/>
+      <c r="AB9" s="4"/>
+      <c r="AC9" s="4"/>
+      <c r="AD9" s="4"/>
+      <c r="AE9" s="4"/>
+      <c r="AF9" s="4"/>
+      <c r="AG9" s="4"/>
+      <c r="AH9" s="4"/>
+      <c r="AI9" s="4"/>
+      <c r="AJ9" s="4"/>
+      <c r="AK9" s="4"/>
+      <c r="AL9" s="17"/>
     </row>
     <row r="10" spans="1:38" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="3">
         <v>45250</v>
       </c>
-      <c r="C10" s="46"/>
-      <c r="D10" s="36"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="42"/>
-      <c r="Q10" s="43"/>
-      <c r="R10" s="44"/>
-      <c r="S10" s="6"/>
-      <c r="T10" s="6"/>
-      <c r="U10" s="6"/>
-      <c r="V10" s="6"/>
-      <c r="W10" s="6"/>
-      <c r="X10" s="6"/>
-      <c r="Y10" s="6"/>
-      <c r="Z10" s="6"/>
-      <c r="AA10" s="6"/>
-      <c r="AB10" s="6"/>
-      <c r="AC10" s="6"/>
-      <c r="AD10" s="6"/>
-      <c r="AE10" s="6"/>
-      <c r="AF10" s="6"/>
-      <c r="AG10" s="6"/>
-      <c r="AH10" s="6"/>
-      <c r="AI10" s="6"/>
-      <c r="AJ10" s="6"/>
-      <c r="AK10" s="6"/>
-      <c r="AL10" s="20"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="47"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="23"/>
+      <c r="Q10" s="24"/>
+      <c r="R10" s="25"/>
+      <c r="S10" s="4"/>
+      <c r="T10" s="4"/>
+      <c r="U10" s="4"/>
+      <c r="V10" s="4"/>
+      <c r="W10" s="4"/>
+      <c r="X10" s="4"/>
+      <c r="Y10" s="4"/>
+      <c r="Z10" s="4"/>
+      <c r="AA10" s="4"/>
+      <c r="AB10" s="4"/>
+      <c r="AC10" s="4"/>
+      <c r="AD10" s="4"/>
+      <c r="AE10" s="4"/>
+      <c r="AF10" s="4"/>
+      <c r="AG10" s="4"/>
+      <c r="AH10" s="4"/>
+      <c r="AI10" s="4"/>
+      <c r="AJ10" s="4"/>
+      <c r="AK10" s="4"/>
+      <c r="AL10" s="17"/>
     </row>
     <row r="11" spans="1:38" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="3">
         <v>45257</v>
       </c>
-      <c r="C11" s="31" t="s">
+      <c r="C11" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="28"/>
-      <c r="F11" s="26" t="s">
+      <c r="D11" s="42"/>
+      <c r="F11" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
-      <c r="P11" s="6"/>
-      <c r="Q11" s="6"/>
-      <c r="R11" s="6"/>
-      <c r="S11" s="39"/>
-      <c r="T11" s="40"/>
-      <c r="U11" s="40"/>
-      <c r="V11" s="41"/>
-      <c r="W11" s="6"/>
-      <c r="X11" s="6"/>
-      <c r="Y11" s="6"/>
-      <c r="Z11" s="6"/>
-      <c r="AA11" s="6"/>
-      <c r="AB11" s="6"/>
-      <c r="AC11" s="6"/>
-      <c r="AD11" s="6"/>
-      <c r="AE11" s="6"/>
-      <c r="AF11" s="6"/>
-      <c r="AG11" s="6"/>
-      <c r="AH11" s="6"/>
-      <c r="AI11" s="6"/>
-      <c r="AJ11" s="6"/>
-      <c r="AK11" s="6"/>
-      <c r="AL11" s="20"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="4"/>
+      <c r="R11" s="4"/>
+      <c r="S11" s="20"/>
+      <c r="T11" s="21"/>
+      <c r="U11" s="21"/>
+      <c r="V11" s="22"/>
+      <c r="W11" s="4"/>
+      <c r="X11" s="4"/>
+      <c r="Y11" s="4"/>
+      <c r="Z11" s="4"/>
+      <c r="AA11" s="4"/>
+      <c r="AB11" s="4"/>
+      <c r="AC11" s="4"/>
+      <c r="AD11" s="4"/>
+      <c r="AE11" s="4"/>
+      <c r="AF11" s="4"/>
+      <c r="AG11" s="4"/>
+      <c r="AH11" s="4"/>
+      <c r="AI11" s="4"/>
+      <c r="AJ11" s="4"/>
+      <c r="AK11" s="4"/>
+      <c r="AL11" s="17"/>
     </row>
     <row r="12" spans="1:38" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="3">
         <v>45264</v>
       </c>
-      <c r="C12" s="32"/>
-      <c r="D12" s="29"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="6"/>
-      <c r="R12" s="6"/>
-      <c r="S12" s="42"/>
-      <c r="T12" s="43"/>
-      <c r="U12" s="43"/>
-      <c r="V12" s="44"/>
-      <c r="W12" s="6"/>
-      <c r="X12" s="6"/>
-      <c r="Y12" s="6"/>
-      <c r="Z12" s="6"/>
-      <c r="AA12" s="6"/>
-      <c r="AB12" s="6"/>
-      <c r="AC12" s="6"/>
-      <c r="AD12" s="6"/>
-      <c r="AE12" s="6"/>
-      <c r="AF12" s="6"/>
-      <c r="AG12" s="6"/>
-      <c r="AH12" s="6"/>
-      <c r="AI12" s="6"/>
-      <c r="AJ12" s="6"/>
-      <c r="AK12" s="6"/>
-      <c r="AL12" s="20"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="43"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="4"/>
+      <c r="S12" s="23"/>
+      <c r="T12" s="24"/>
+      <c r="U12" s="24"/>
+      <c r="V12" s="25"/>
+      <c r="W12" s="4"/>
+      <c r="X12" s="4"/>
+      <c r="Y12" s="4"/>
+      <c r="Z12" s="4"/>
+      <c r="AA12" s="4"/>
+      <c r="AB12" s="4"/>
+      <c r="AC12" s="4"/>
+      <c r="AD12" s="4"/>
+      <c r="AE12" s="4"/>
+      <c r="AF12" s="4"/>
+      <c r="AG12" s="4"/>
+      <c r="AH12" s="4"/>
+      <c r="AI12" s="4"/>
+      <c r="AJ12" s="4"/>
+      <c r="AK12" s="4"/>
+      <c r="AL12" s="17"/>
     </row>
     <row r="13" spans="1:38" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="3">
         <v>45271</v>
       </c>
-      <c r="C13" s="33"/>
-      <c r="D13" s="30"/>
-      <c r="F13" s="26" t="s">
+      <c r="C13" s="32"/>
+      <c r="D13" s="44"/>
+      <c r="F13" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
-      <c r="M13" s="6"/>
-      <c r="N13" s="6"/>
-      <c r="O13" s="6"/>
-      <c r="P13" s="6"/>
-      <c r="Q13" s="6"/>
-      <c r="R13" s="6"/>
-      <c r="S13" s="6"/>
-      <c r="T13" s="6"/>
-      <c r="U13" s="6"/>
-      <c r="V13" s="6"/>
-      <c r="W13" s="39"/>
-      <c r="X13" s="40"/>
-      <c r="Y13" s="40"/>
-      <c r="Z13" s="40"/>
-      <c r="AA13" s="41"/>
-      <c r="AB13" s="6"/>
-      <c r="AC13" s="6"/>
-      <c r="AD13" s="6"/>
-      <c r="AE13" s="6"/>
-      <c r="AF13" s="6"/>
-      <c r="AG13" s="6"/>
-      <c r="AH13" s="6"/>
-      <c r="AI13" s="6"/>
-      <c r="AJ13" s="6"/>
-      <c r="AK13" s="6"/>
-      <c r="AL13" s="20"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
+      <c r="R13" s="4"/>
+      <c r="S13" s="4"/>
+      <c r="T13" s="4"/>
+      <c r="U13" s="4"/>
+      <c r="V13" s="4"/>
+      <c r="W13" s="20"/>
+      <c r="X13" s="21"/>
+      <c r="Y13" s="21"/>
+      <c r="Z13" s="21"/>
+      <c r="AA13" s="22"/>
+      <c r="AB13" s="4"/>
+      <c r="AC13" s="4"/>
+      <c r="AD13" s="4"/>
+      <c r="AE13" s="4"/>
+      <c r="AF13" s="4"/>
+      <c r="AG13" s="4"/>
+      <c r="AH13" s="4"/>
+      <c r="AI13" s="4"/>
+      <c r="AJ13" s="4"/>
+      <c r="AK13" s="4"/>
+      <c r="AL13" s="17"/>
     </row>
     <row r="14" spans="1:38" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="3">
         <v>45278</v>
       </c>
-      <c r="C14" s="31" t="s">
+      <c r="C14" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="34"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="6"/>
-      <c r="O14" s="6"/>
-      <c r="P14" s="6"/>
-      <c r="Q14" s="6"/>
-      <c r="R14" s="6"/>
-      <c r="S14" s="6"/>
-      <c r="T14" s="6"/>
-      <c r="U14" s="6"/>
-      <c r="V14" s="6"/>
-      <c r="W14" s="42"/>
-      <c r="X14" s="43"/>
-      <c r="Y14" s="43"/>
-      <c r="Z14" s="43"/>
-      <c r="AA14" s="44"/>
-      <c r="AB14" s="6"/>
-      <c r="AC14" s="6"/>
-      <c r="AD14" s="6"/>
-      <c r="AE14" s="6"/>
-      <c r="AF14" s="6"/>
-      <c r="AG14" s="6"/>
-      <c r="AH14" s="6"/>
-      <c r="AI14" s="6"/>
-      <c r="AJ14" s="6"/>
-      <c r="AK14" s="6"/>
-      <c r="AL14" s="20"/>
+      <c r="D14" s="45"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4"/>
+      <c r="R14" s="4"/>
+      <c r="S14" s="4"/>
+      <c r="T14" s="4"/>
+      <c r="U14" s="4"/>
+      <c r="V14" s="4"/>
+      <c r="W14" s="23"/>
+      <c r="X14" s="24"/>
+      <c r="Y14" s="24"/>
+      <c r="Z14" s="24"/>
+      <c r="AA14" s="25"/>
+      <c r="AB14" s="4"/>
+      <c r="AC14" s="4"/>
+      <c r="AD14" s="4"/>
+      <c r="AE14" s="4"/>
+      <c r="AF14" s="4"/>
+      <c r="AG14" s="4"/>
+      <c r="AH14" s="4"/>
+      <c r="AI14" s="4"/>
+      <c r="AJ14" s="4"/>
+      <c r="AK14" s="4"/>
+      <c r="AL14" s="17"/>
     </row>
     <row r="15" spans="1:38" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="3">
         <v>45285</v>
       </c>
-      <c r="C15" s="32"/>
-      <c r="D15" s="35"/>
-      <c r="F15" s="45" t="s">
+      <c r="C15" s="31"/>
+      <c r="D15" s="46"/>
+      <c r="F15" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="39"/>
-      <c r="L15" s="40"/>
-      <c r="M15" s="40"/>
-      <c r="N15" s="40"/>
-      <c r="O15" s="40"/>
-      <c r="P15" s="40"/>
-      <c r="Q15" s="40"/>
-      <c r="R15" s="40"/>
-      <c r="S15" s="40"/>
-      <c r="T15" s="40"/>
-      <c r="U15" s="40"/>
-      <c r="V15" s="40"/>
-      <c r="W15" s="40"/>
-      <c r="X15" s="40"/>
-      <c r="Y15" s="40"/>
-      <c r="Z15" s="40"/>
-      <c r="AA15" s="40"/>
-      <c r="AB15" s="40"/>
-      <c r="AC15" s="40"/>
-      <c r="AD15" s="40"/>
-      <c r="AE15" s="41"/>
-      <c r="AF15" s="6"/>
-      <c r="AG15" s="6"/>
-      <c r="AH15" s="6"/>
-      <c r="AI15" s="6"/>
-      <c r="AJ15" s="6"/>
-      <c r="AK15" s="6"/>
-      <c r="AL15" s="20"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="20"/>
+      <c r="L15" s="21"/>
+      <c r="M15" s="21"/>
+      <c r="N15" s="21"/>
+      <c r="O15" s="21"/>
+      <c r="P15" s="21"/>
+      <c r="Q15" s="21"/>
+      <c r="R15" s="21"/>
+      <c r="S15" s="21"/>
+      <c r="T15" s="21"/>
+      <c r="U15" s="21"/>
+      <c r="V15" s="21"/>
+      <c r="W15" s="21"/>
+      <c r="X15" s="21"/>
+      <c r="Y15" s="21"/>
+      <c r="Z15" s="21"/>
+      <c r="AA15" s="21"/>
+      <c r="AB15" s="21"/>
+      <c r="AC15" s="21"/>
+      <c r="AD15" s="21"/>
+      <c r="AE15" s="22"/>
+      <c r="AF15" s="4"/>
+      <c r="AG15" s="4"/>
+      <c r="AH15" s="4"/>
+      <c r="AI15" s="4"/>
+      <c r="AJ15" s="4"/>
+      <c r="AK15" s="4"/>
+      <c r="AL15" s="17"/>
     </row>
     <row r="16" spans="1:38" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="3">
         <v>45292</v>
       </c>
-      <c r="C16" s="32"/>
-      <c r="D16" s="35"/>
-      <c r="F16" s="45"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="42"/>
-      <c r="L16" s="43"/>
-      <c r="M16" s="43"/>
-      <c r="N16" s="43"/>
-      <c r="O16" s="43"/>
-      <c r="P16" s="43"/>
-      <c r="Q16" s="43"/>
-      <c r="R16" s="43"/>
-      <c r="S16" s="43"/>
-      <c r="T16" s="43"/>
-      <c r="U16" s="43"/>
-      <c r="V16" s="43"/>
-      <c r="W16" s="43"/>
-      <c r="X16" s="43"/>
-      <c r="Y16" s="43"/>
-      <c r="Z16" s="43"/>
-      <c r="AA16" s="43"/>
-      <c r="AB16" s="43"/>
-      <c r="AC16" s="43"/>
-      <c r="AD16" s="43"/>
-      <c r="AE16" s="44"/>
-      <c r="AF16" s="6"/>
-      <c r="AG16" s="6"/>
-      <c r="AH16" s="6"/>
-      <c r="AI16" s="6"/>
-      <c r="AJ16" s="6"/>
-      <c r="AK16" s="6"/>
-      <c r="AL16" s="20"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="46"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="23"/>
+      <c r="L16" s="24"/>
+      <c r="M16" s="24"/>
+      <c r="N16" s="24"/>
+      <c r="O16" s="24"/>
+      <c r="P16" s="24"/>
+      <c r="Q16" s="24"/>
+      <c r="R16" s="24"/>
+      <c r="S16" s="24"/>
+      <c r="T16" s="24"/>
+      <c r="U16" s="24"/>
+      <c r="V16" s="24"/>
+      <c r="W16" s="24"/>
+      <c r="X16" s="24"/>
+      <c r="Y16" s="24"/>
+      <c r="Z16" s="24"/>
+      <c r="AA16" s="24"/>
+      <c r="AB16" s="24"/>
+      <c r="AC16" s="24"/>
+      <c r="AD16" s="24"/>
+      <c r="AE16" s="25"/>
+      <c r="AF16" s="4"/>
+      <c r="AG16" s="4"/>
+      <c r="AH16" s="4"/>
+      <c r="AI16" s="4"/>
+      <c r="AJ16" s="4"/>
+      <c r="AK16" s="4"/>
+      <c r="AL16" s="17"/>
     </row>
     <row r="17" spans="1:38" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17" s="3">
         <v>45299</v>
       </c>
-      <c r="C17" s="33"/>
-      <c r="D17" s="36"/>
-      <c r="F17" s="26" t="s">
+      <c r="C17" s="32"/>
+      <c r="D17" s="47"/>
+      <c r="F17" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
-      <c r="M17" s="6"/>
-      <c r="N17" s="6"/>
-      <c r="O17" s="6"/>
-      <c r="P17" s="6"/>
-      <c r="Q17" s="6"/>
-      <c r="R17" s="6"/>
-      <c r="S17" s="6"/>
-      <c r="T17" s="6"/>
-      <c r="U17" s="6"/>
-      <c r="V17" s="6"/>
-      <c r="W17" s="6"/>
-      <c r="X17" s="6"/>
-      <c r="Y17" s="6"/>
-      <c r="Z17" s="6"/>
-      <c r="AA17" s="6"/>
-      <c r="AB17" s="6"/>
-      <c r="AC17" s="6"/>
-      <c r="AD17" s="6"/>
-      <c r="AE17" s="6"/>
-      <c r="AF17" s="39"/>
-      <c r="AG17" s="40"/>
-      <c r="AH17" s="40"/>
-      <c r="AI17" s="40"/>
-      <c r="AJ17" s="40"/>
-      <c r="AK17" s="41"/>
-      <c r="AL17" s="20"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="4"/>
+      <c r="Q17" s="4"/>
+      <c r="R17" s="4"/>
+      <c r="S17" s="4"/>
+      <c r="T17" s="4"/>
+      <c r="U17" s="4"/>
+      <c r="V17" s="4"/>
+      <c r="W17" s="4"/>
+      <c r="X17" s="4"/>
+      <c r="Y17" s="4"/>
+      <c r="Z17" s="4"/>
+      <c r="AA17" s="4"/>
+      <c r="AB17" s="4"/>
+      <c r="AC17" s="4"/>
+      <c r="AD17" s="4"/>
+      <c r="AE17" s="4"/>
+      <c r="AF17" s="20"/>
+      <c r="AG17" s="21"/>
+      <c r="AH17" s="21"/>
+      <c r="AI17" s="21"/>
+      <c r="AJ17" s="21"/>
+      <c r="AK17" s="22"/>
+      <c r="AL17" s="17"/>
     </row>
     <row r="18" spans="1:38" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="3">
         <v>45306</v>
       </c>
-      <c r="C18" s="31" t="s">
+      <c r="C18" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="23"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="6"/>
-      <c r="M18" s="6"/>
-      <c r="N18" s="6"/>
-      <c r="O18" s="6"/>
-      <c r="P18" s="6"/>
-      <c r="Q18" s="6"/>
-      <c r="R18" s="6"/>
-      <c r="S18" s="6"/>
-      <c r="T18" s="6"/>
-      <c r="U18" s="6"/>
-      <c r="V18" s="6"/>
-      <c r="W18" s="6"/>
-      <c r="X18" s="6"/>
-      <c r="Y18" s="6"/>
-      <c r="Z18" s="6"/>
-      <c r="AA18" s="6"/>
-      <c r="AB18" s="6"/>
-      <c r="AC18" s="6"/>
-      <c r="AD18" s="6"/>
-      <c r="AE18" s="6"/>
-      <c r="AF18" s="42"/>
-      <c r="AG18" s="43"/>
-      <c r="AH18" s="43"/>
-      <c r="AI18" s="43"/>
-      <c r="AJ18" s="43"/>
-      <c r="AK18" s="44"/>
-      <c r="AL18" s="20"/>
+      <c r="D18" s="48"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="4"/>
+      <c r="R18" s="4"/>
+      <c r="S18" s="4"/>
+      <c r="T18" s="4"/>
+      <c r="U18" s="4"/>
+      <c r="V18" s="4"/>
+      <c r="W18" s="4"/>
+      <c r="X18" s="4"/>
+      <c r="Y18" s="4"/>
+      <c r="Z18" s="4"/>
+      <c r="AA18" s="4"/>
+      <c r="AB18" s="4"/>
+      <c r="AC18" s="4"/>
+      <c r="AD18" s="4"/>
+      <c r="AE18" s="4"/>
+      <c r="AF18" s="23"/>
+      <c r="AG18" s="24"/>
+      <c r="AH18" s="24"/>
+      <c r="AI18" s="24"/>
+      <c r="AJ18" s="24"/>
+      <c r="AK18" s="25"/>
+      <c r="AL18" s="17"/>
     </row>
     <row r="19" spans="1:38" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B19" s="3">
         <v>45313</v>
       </c>
-      <c r="C19" s="32"/>
-      <c r="D19" s="24"/>
-      <c r="F19" s="26" t="s">
+      <c r="C19" s="31"/>
+      <c r="D19" s="49"/>
+      <c r="F19" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
-      <c r="M19" s="6"/>
-      <c r="N19" s="6"/>
-      <c r="O19" s="6"/>
-      <c r="P19" s="6"/>
-      <c r="Q19" s="6"/>
-      <c r="R19" s="6"/>
-      <c r="S19" s="6"/>
-      <c r="T19" s="6"/>
-      <c r="U19" s="6"/>
-      <c r="V19" s="6"/>
-      <c r="W19" s="6"/>
-      <c r="X19" s="6"/>
-      <c r="Y19" s="6"/>
-      <c r="Z19" s="6"/>
-      <c r="AA19" s="6"/>
-      <c r="AB19" s="6"/>
-      <c r="AC19" s="6"/>
-      <c r="AD19" s="6"/>
-      <c r="AE19" s="6"/>
-      <c r="AF19" s="6"/>
-      <c r="AG19" s="6"/>
-      <c r="AH19" s="6"/>
-      <c r="AI19" s="6"/>
-      <c r="AJ19" s="6"/>
-      <c r="AK19" s="6"/>
-      <c r="AL19" s="47"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="4"/>
+      <c r="R19" s="4"/>
+      <c r="S19" s="4"/>
+      <c r="T19" s="4"/>
+      <c r="U19" s="4"/>
+      <c r="V19" s="4"/>
+      <c r="W19" s="4"/>
+      <c r="X19" s="4"/>
+      <c r="Y19" s="4"/>
+      <c r="Z19" s="4"/>
+      <c r="AA19" s="4"/>
+      <c r="AB19" s="4"/>
+      <c r="AC19" s="4"/>
+      <c r="AD19" s="4"/>
+      <c r="AE19" s="4"/>
+      <c r="AF19" s="4"/>
+      <c r="AG19" s="4"/>
+      <c r="AH19" s="4"/>
+      <c r="AI19" s="4"/>
+      <c r="AJ19" s="4"/>
+      <c r="AK19" s="4"/>
+      <c r="AL19" s="26"/>
     </row>
     <row r="20" spans="1:38" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B20" s="3">
         <v>45320</v>
       </c>
-      <c r="C20" s="32"/>
-      <c r="D20" s="24"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
-      <c r="K20" s="22"/>
-      <c r="L20" s="22"/>
-      <c r="M20" s="22"/>
-      <c r="N20" s="22"/>
-      <c r="O20" s="22"/>
-      <c r="P20" s="22"/>
-      <c r="Q20" s="22"/>
-      <c r="R20" s="22"/>
-      <c r="S20" s="22"/>
-      <c r="T20" s="22"/>
-      <c r="U20" s="22"/>
-      <c r="V20" s="22"/>
-      <c r="W20" s="22"/>
-      <c r="X20" s="22"/>
-      <c r="Y20" s="22"/>
-      <c r="Z20" s="22"/>
-      <c r="AA20" s="22"/>
-      <c r="AB20" s="22"/>
-      <c r="AC20" s="22"/>
-      <c r="AD20" s="22"/>
-      <c r="AE20" s="22"/>
-      <c r="AF20" s="22"/>
-      <c r="AG20" s="22"/>
-      <c r="AH20" s="22"/>
-      <c r="AI20" s="22"/>
-      <c r="AJ20" s="22"/>
-      <c r="AK20" s="22"/>
-      <c r="AL20" s="48"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="49"/>
+      <c r="F20" s="36"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="19"/>
+      <c r="K20" s="19"/>
+      <c r="L20" s="19"/>
+      <c r="M20" s="19"/>
+      <c r="N20" s="19"/>
+      <c r="O20" s="19"/>
+      <c r="P20" s="19"/>
+      <c r="Q20" s="19"/>
+      <c r="R20" s="19"/>
+      <c r="S20" s="19"/>
+      <c r="T20" s="19"/>
+      <c r="U20" s="19"/>
+      <c r="V20" s="19"/>
+      <c r="W20" s="19"/>
+      <c r="X20" s="19"/>
+      <c r="Y20" s="19"/>
+      <c r="Z20" s="19"/>
+      <c r="AA20" s="19"/>
+      <c r="AB20" s="19"/>
+      <c r="AC20" s="19"/>
+      <c r="AD20" s="19"/>
+      <c r="AE20" s="19"/>
+      <c r="AF20" s="19"/>
+      <c r="AG20" s="19"/>
+      <c r="AH20" s="19"/>
+      <c r="AI20" s="19"/>
+      <c r="AJ20" s="19"/>
+      <c r="AK20" s="19"/>
+      <c r="AL20" s="27"/>
     </row>
     <row r="21" spans="1:38" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B21" s="3">
         <v>45327</v>
       </c>
-      <c r="C21" s="32"/>
-      <c r="D21" s="24"/>
-      <c r="F21" s="7"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="49"/>
+      <c r="F21" s="5"/>
     </row>
     <row r="22" spans="1:38" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="4">
+      <c r="B22" s="3">
         <v>45334</v>
       </c>
-      <c r="C22" s="33"/>
-      <c r="D22" s="25"/>
-      <c r="F22" s="7"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="50"/>
+      <c r="F22" s="5"/>
     </row>
     <row r="23" spans="1:38" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="4">
+      <c r="B23" s="3">
         <v>45341</v>
       </c>
-      <c r="C23" s="31" t="s">
+      <c r="C23" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="D23" s="34"/>
-      <c r="F23" s="7" t="s">
+      <c r="D23" s="45"/>
+      <c r="F23" s="5" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:38" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="4">
+      <c r="B24" s="3">
         <v>45348</v>
       </c>
-      <c r="C24" s="32"/>
-      <c r="D24" s="35"/>
-      <c r="F24" s="7"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="46"/>
+      <c r="F24" s="5"/>
     </row>
     <row r="25" spans="1:38" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="4">
+      <c r="B25" s="3">
         <v>45355</v>
       </c>
-      <c r="C25" s="32"/>
-      <c r="D25" s="35"/>
-      <c r="F25" s="7"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="46"/>
+      <c r="F25" s="5"/>
     </row>
     <row r="26" spans="1:38" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="4">
+      <c r="B26" s="3">
         <v>45362</v>
       </c>
-      <c r="C26" s="33"/>
-      <c r="D26" s="36"/>
-      <c r="F26" s="7"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="47"/>
+      <c r="F26" s="5"/>
     </row>
     <row r="27" spans="1:38" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="4">
+      <c r="B27" s="3">
         <v>45369</v>
       </c>
-      <c r="C27" s="31" t="s">
+      <c r="C27" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="D27" s="28"/>
+      <c r="D27" s="42"/>
     </row>
     <row r="28" spans="1:38" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="B28" s="4">
+      <c r="B28" s="3">
         <v>45376</v>
       </c>
-      <c r="C28" s="32"/>
-      <c r="D28" s="29"/>
+      <c r="C28" s="31"/>
+      <c r="D28" s="43"/>
     </row>
     <row r="29" spans="1:38" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="B29" s="4">
+      <c r="B29" s="3">
         <v>45383</v>
       </c>
-      <c r="C29" s="32"/>
-      <c r="D29" s="29"/>
-      <c r="F29" s="7"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="43"/>
+      <c r="F29" s="5"/>
     </row>
     <row r="30" spans="1:38" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="B30" s="4">
+      <c r="B30" s="3">
         <v>45390</v>
       </c>
-      <c r="C30" s="32"/>
-      <c r="D30" s="29"/>
-      <c r="F30" s="7"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="43"/>
+      <c r="F30" s="5"/>
     </row>
     <row r="31" spans="1:38" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="B31" s="4">
+      <c r="B31" s="3">
         <v>45397</v>
       </c>
-      <c r="C31" s="32"/>
-      <c r="D31" s="29"/>
-      <c r="F31" s="7"/>
+      <c r="C31" s="31"/>
+      <c r="D31" s="43"/>
+      <c r="F31" s="5"/>
     </row>
     <row r="32" spans="1:38" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="B32" s="4">
+      <c r="B32" s="3">
         <v>45404</v>
       </c>
-      <c r="C32" s="33"/>
-      <c r="D32" s="30"/>
-      <c r="F32" s="7"/>
-    </row>
-    <row r="33" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+      <c r="C32" s="32"/>
+      <c r="D32" s="44"/>
+      <c r="F32" s="5"/>
+    </row>
+    <row r="33" spans="1:6" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="B33" s="4">
+      <c r="B33" s="52">
         <v>45411</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="D33" s="5"/>
-      <c r="F33" s="7"/>
+      <c r="D33" s="54"/>
+      <c r="F33" s="5"/>
     </row>
     <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F34" s="7"/>
+      <c r="F34" s="5"/>
     </row>
     <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F35" s="7"/>
+      <c r="F35" s="5"/>
     </row>
     <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F37" s="7"/>
+      <c r="F37" s="5"/>
     </row>
     <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F38" s="7"/>
+      <c r="F38" s="5"/>
     </row>
     <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F39" s="7"/>
+      <c r="F39" s="5"/>
     </row>
     <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F40" s="7"/>
+      <c r="F40" s="5"/>
     </row>
     <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F41" s="7"/>
+      <c r="F41" s="5"/>
     </row>
     <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="AF17:AK18"/>
-    <mergeCell ref="AL19:AL20"/>
-    <mergeCell ref="S11:V12"/>
-    <mergeCell ref="W13:AA14"/>
-    <mergeCell ref="K15:AE16"/>
+    <mergeCell ref="D18:D22"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="D27:D32"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="D3:D5"/>
+    <mergeCell ref="D6:D10"/>
+    <mergeCell ref="D11:D13"/>
+    <mergeCell ref="D14:D17"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="K7:O8"/>
     <mergeCell ref="P9:R10"/>
@@ -2276,16 +2338,11 @@
     <mergeCell ref="D23:D26"/>
     <mergeCell ref="C3:C5"/>
     <mergeCell ref="C6:C10"/>
-    <mergeCell ref="D18:D22"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="D27:D32"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="C14:C17"/>
-    <mergeCell ref="D3:D5"/>
-    <mergeCell ref="D6:D10"/>
-    <mergeCell ref="D11:D13"/>
-    <mergeCell ref="D14:D17"/>
+    <mergeCell ref="AF17:AK18"/>
+    <mergeCell ref="AL19:AL20"/>
+    <mergeCell ref="S11:V12"/>
+    <mergeCell ref="W13:AA14"/>
+    <mergeCell ref="K15:AE16"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>